<commit_message>
updated vitae and add tidytuesday plot
</commit_message>
<xml_diff>
--- a/khurana_cv/data/courses_taught.xlsx
+++ b/khurana_cv/data/courses_taught.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havis\University of Oregon Dropbox\Havi Khurana\Personal\Coding projects\khurana_cv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692B52F3-D81E-4F72-8277-56B97E8CF6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9190CC18-AFAD-4ABB-A787-4A3E97141BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{F4143829-AF9E-244C-8EFD-6252778B5E60}"/>
   </bookViews>
@@ -161,17 +161,17 @@
     <t>EDUC 641/643/645: Applied Statistics in Education and Human Services (Discussion Session)</t>
   </si>
   <si>
+    <t>2022-24</t>
+  </si>
+  <si>
+    <t>2017-19</t>
+  </si>
+  <si>
     <t>Led lab sessions introducing R programming langugage to run, analyze, and communicate results from common statistical models
 Developed learning material (worksheets) for student practice and summarizing concepts
-Supervised a team of 2-3 GEs
+Supervised a team of graduate employees
 Held virtual and in-person office hours for answering students' questions
 Graded student assignment and provided feedback through a rubric</t>
-  </si>
-  <si>
-    <t>2022-24</t>
-  </si>
-  <si>
-    <t>2017-19</t>
   </si>
 </sst>
 </file>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80AB2D6-D787-8D4A-BD11-32CAE09CA316}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="I2" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -614,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -644,7 +644,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="31">
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>

</xml_diff>